<commit_message>
correcting ass in minimum criteria
</commit_message>
<xml_diff>
--- a/results/Results_DF.xlsx
+++ b/results/Results_DF.xlsx
@@ -2576,49 +2576,49 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>70.2482638888889</v>
       </c>
       <c r="I2" t="n">
         <v>0.2776407693384201</v>
       </c>
       <c r="J2" t="n">
-        <v>50</v>
+        <v>69.69481646825398</v>
       </c>
       <c r="K2" t="n">
         <v>0.2707586358251031</v>
       </c>
       <c r="L2" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="M2" t="n">
         <v>0.07932692307692307</v>
       </c>
       <c r="N2" t="n">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="O2" t="n">
         <v>0.00686695278969957</v>
       </c>
       <c r="P2" t="n">
-        <v>50</v>
+        <v>96.5</v>
       </c>
       <c r="Q2" t="n">
         <v>0.6279545454545454</v>
       </c>
       <c r="R2" t="n">
-        <v>50</v>
+        <v>99.5</v>
       </c>
       <c r="S2" t="n">
         <v>0.5747365841705464</v>
       </c>
       <c r="T2" t="n">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="U2" t="n">
         <v>0.2570711678832117</v>
       </c>
       <c r="V2" t="n">
-        <v>50</v>
+        <v>69.33333333333333</v>
       </c>
       <c r="W2" t="n">
         <v>0.2647245288983469</v>

</xml_diff>